<commit_message>
Added i2c1 pin setup.
</commit_message>
<xml_diff>
--- a/Sitara Pinout.xlsx
+++ b/Sitara Pinout.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="814">
   <si>
     <t>Pin #</t>
   </si>
@@ -2161,12 +2161,6 @@
     <t>conf_spi0_d1</t>
   </si>
   <si>
-    <t>0x62</t>
-  </si>
-  <si>
-    <t>no change - init in uboot by neal, slew=slow,I/O,pulldown,mode=2</t>
-  </si>
-  <si>
     <t>conf_gpmc_ad13</t>
   </si>
   <si>
@@ -2468,6 +2462,12 @@
   </si>
   <si>
     <t>no change. Kernel panic on boot (capemgr crashing?) without i2c2, not sure why. Peek = 0x73</t>
+  </si>
+  <si>
+    <t>slew=fast,I/O,pull disabled,mode=7</t>
+  </si>
+  <si>
+    <t>init in uboot by neal, reinit in device tree, slew=fast,I/O,pull disabled,mode=2</t>
   </si>
 </sst>
 </file>
@@ -2531,7 +2531,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2628,6 +2628,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2775,7 +2781,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3043,6 +3049,21 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -3330,10 +3351,10 @@
   <dimension ref="A1:V115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U88" sqref="U88"/>
+      <selection pane="bottomRight" activeCell="T54" sqref="T54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3381,16 +3402,16 @@
         <v>4</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>773</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>775</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>774</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>777</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>5</v>
@@ -3510,7 +3531,7 @@
         <v>96</v>
       </c>
       <c r="T3" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -3561,7 +3582,7 @@
         <v>97</v>
       </c>
       <c r="T4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -4299,7 +4320,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="15"/>
       <c r="M19" s="16" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="N19" s="16" t="s">
         <v>608</v>
@@ -4383,7 +4404,7 @@
         <v>70</v>
       </c>
       <c r="T20" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -4447,7 +4468,7 @@
         <v>71</v>
       </c>
       <c r="T21" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -4511,7 +4532,7 @@
         <v>72</v>
       </c>
       <c r="T22" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -4575,7 +4596,7 @@
         <v>73</v>
       </c>
       <c r="T23" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -4639,7 +4660,7 @@
         <v>74</v>
       </c>
       <c r="T24" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -4703,7 +4724,7 @@
         <v>75</v>
       </c>
       <c r="T25" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -4767,7 +4788,7 @@
         <v>76</v>
       </c>
       <c r="T26" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -4831,7 +4852,7 @@
         <v>77</v>
       </c>
       <c r="T27" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -4895,7 +4916,7 @@
         <v>78</v>
       </c>
       <c r="T28" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -4959,7 +4980,7 @@
         <v>79</v>
       </c>
       <c r="T29" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -5023,7 +5044,7 @@
         <v>80</v>
       </c>
       <c r="T30" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -5087,7 +5108,7 @@
         <v>81</v>
       </c>
       <c r="T31" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -5151,7 +5172,7 @@
         <v>8</v>
       </c>
       <c r="T32" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
@@ -5215,7 +5236,7 @@
         <v>9</v>
       </c>
       <c r="T33" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -5279,7 +5300,7 @@
         <v>10</v>
       </c>
       <c r="T34" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
@@ -5343,7 +5364,7 @@
         <v>11</v>
       </c>
       <c r="T35" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
@@ -5407,7 +5428,7 @@
         <v>86</v>
       </c>
       <c r="T36" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -5471,7 +5492,7 @@
         <v>87</v>
       </c>
       <c r="T37" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
@@ -5535,7 +5556,7 @@
         <v>88</v>
       </c>
       <c r="T38" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
@@ -5596,7 +5617,7 @@
         <v>89</v>
       </c>
       <c r="T39" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -5659,7 +5680,7 @@
         <v>114</v>
       </c>
       <c r="T40" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -5848,7 +5869,7 @@
         <v>117</v>
       </c>
       <c r="T43" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -5988,7 +6009,7 @@
         <v>548</v>
       </c>
       <c r="G46" s="39" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="H46" s="39">
         <v>0</v>
@@ -6260,28 +6281,40 @@
       <c r="E51" s="14">
         <v>1</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F51" s="95" t="s">
         <v>549</v>
       </c>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="M51" s="12" t="s">
+      <c r="H51" s="95">
+        <v>1</v>
+      </c>
+      <c r="I51" s="95">
+        <v>1</v>
+      </c>
+      <c r="J51" s="95">
+        <v>0</v>
+      </c>
+      <c r="K51" s="95">
+        <v>1</v>
+      </c>
+      <c r="L51" s="96">
+        <v>2</v>
+      </c>
+      <c r="M51" s="97" t="s">
         <v>591</v>
       </c>
-      <c r="N51" s="12" t="s">
+      <c r="N51" s="97" t="s">
         <v>693</v>
       </c>
-      <c r="O51" s="52" t="str">
+      <c r="O51" s="98" t="str">
         <f t="shared" si="3"/>
         <v>15C</v>
       </c>
-      <c r="P51" s="61" t="s">
-        <v>711</v>
+      <c r="P51" s="99" t="str">
+        <f t="shared" ref="P51:P57" si="7">CONCATENATE("0x",DEC2HEX(H51*64 + I51*32 + J51*16 +K51*8 + L51,2))</f>
+        <v>0x6A</v>
       </c>
       <c r="Q51" s="57">
         <f t="shared" si="2"/>
@@ -6292,7 +6325,7 @@
         <v>5</v>
       </c>
       <c r="T51" t="s">
-        <v>712</v>
+        <v>813</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
@@ -6322,7 +6355,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="M52" s="12" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N52" s="12">
         <v>960</v>
@@ -6343,7 +6376,7 @@
         <v>6</v>
       </c>
       <c r="T52" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
@@ -6394,7 +6427,7 @@
         <v>154</v>
       </c>
       <c r="P53" s="64" t="str">
-        <f t="shared" ref="P53:P57" si="7">CONCATENATE("0x",DEC2HEX(H53*64 + I53*32 + J53*16 +K53*8 + L53,2))</f>
+        <f t="shared" si="7"/>
         <v>0x27</v>
       </c>
       <c r="Q53" s="57">
@@ -6406,7 +6439,7 @@
         <v>3</v>
       </c>
       <c r="T53" t="s">
-        <v>707</v>
+        <v>812</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
@@ -6425,28 +6458,40 @@
       <c r="E54" s="14">
         <v>2</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" s="95" t="s">
         <v>549</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="95" t="s">
         <v>184</v>
       </c>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="M54" s="12" t="s">
+      <c r="H54" s="95">
+        <v>1</v>
+      </c>
+      <c r="I54" s="95">
+        <v>1</v>
+      </c>
+      <c r="J54" s="95">
+        <v>0</v>
+      </c>
+      <c r="K54" s="95">
+        <v>1</v>
+      </c>
+      <c r="L54" s="96">
+        <v>2</v>
+      </c>
+      <c r="M54" s="97" t="s">
         <v>710</v>
       </c>
-      <c r="N54" s="12">
+      <c r="N54" s="97">
         <v>958</v>
       </c>
-      <c r="O54" s="52" t="str">
+      <c r="O54" s="98" t="str">
         <f t="shared" si="3"/>
         <v>158</v>
       </c>
-      <c r="P54" s="61" t="s">
-        <v>711</v>
+      <c r="P54" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>0x6A</v>
       </c>
       <c r="Q54" s="57">
         <f t="shared" si="2"/>
@@ -6457,7 +6502,7 @@
         <v>4</v>
       </c>
       <c r="T54" t="s">
-        <v>712</v>
+        <v>813</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
@@ -6549,7 +6594,7 @@
       <c r="K56" s="8"/>
       <c r="L56" s="9"/>
       <c r="M56" s="13" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="N56" s="13">
         <v>968</v>
@@ -6559,7 +6604,7 @@
         <v>168</v>
       </c>
       <c r="P56" s="65" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="Q56" s="57">
         <f t="shared" si="2"/>
@@ -6571,7 +6616,7 @@
       </c>
       <c r="S56"/>
       <c r="T56" s="7" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="57" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -6786,7 +6831,7 @@
         <v>178</v>
       </c>
       <c r="P60" s="61" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="Q60" s="57">
         <f t="shared" si="2"/>
@@ -6797,7 +6842,7 @@
         <v>12</v>
       </c>
       <c r="T60" s="71" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
@@ -6848,7 +6893,7 @@
         <v>17C</v>
       </c>
       <c r="P61" s="61" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="Q61" s="57">
         <f t="shared" si="2"/>
@@ -6859,7 +6904,7 @@
         <v>13</v>
       </c>
       <c r="T61" s="71" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
@@ -8085,7 +8130,7 @@
         <v>1</v>
       </c>
       <c r="M82" s="12" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="N82" s="12">
         <v>800</v>
@@ -8095,7 +8140,7 @@
         <v>0</v>
       </c>
       <c r="P82" s="59" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="Q82" s="57">
         <f t="shared" si="10"/>
@@ -8106,7 +8151,7 @@
         <v>32</v>
       </c>
       <c r="T82" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
@@ -8139,7 +8184,7 @@
         <v>1</v>
       </c>
       <c r="M83" s="12" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="N83" s="12">
         <v>804</v>
@@ -8149,7 +8194,7 @@
         <v>4</v>
       </c>
       <c r="P83" s="59" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="Q83" s="57">
         <f t="shared" si="10"/>
@@ -8160,7 +8205,7 @@
         <v>33</v>
       </c>
       <c r="T83" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
@@ -8193,7 +8238,7 @@
         <v>1</v>
       </c>
       <c r="M84" s="12" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="N84" s="12">
         <v>808</v>
@@ -8203,7 +8248,7 @@
         <v>8</v>
       </c>
       <c r="P84" s="59" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="Q84" s="57">
         <f t="shared" si="10"/>
@@ -8214,7 +8259,7 @@
         <v>34</v>
       </c>
       <c r="T84" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
@@ -8247,17 +8292,17 @@
         <v>1</v>
       </c>
       <c r="M85" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="N85" s="12" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="O85" s="52" t="str">
         <f t="shared" si="12"/>
         <v>C</v>
       </c>
       <c r="P85" s="59" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="Q85" s="57">
         <f t="shared" si="10"/>
@@ -8268,7 +8313,7 @@
         <v>35</v>
       </c>
       <c r="T85" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
@@ -8301,7 +8346,7 @@
         <v>1</v>
       </c>
       <c r="M86" s="12" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="N86" s="12">
         <v>810</v>
@@ -8311,7 +8356,7 @@
         <v>10</v>
       </c>
       <c r="P86" s="59" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="Q86" s="57">
         <f t="shared" si="10"/>
@@ -8322,7 +8367,7 @@
         <v>36</v>
       </c>
       <c r="T86" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
@@ -8355,7 +8400,7 @@
         <v>1</v>
       </c>
       <c r="M87" s="12" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N87" s="12">
         <v>814</v>
@@ -8365,7 +8410,7 @@
         <v>14</v>
       </c>
       <c r="P87" s="59" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="Q87" s="57">
         <f t="shared" si="10"/>
@@ -8376,7 +8421,7 @@
         <v>37</v>
       </c>
       <c r="T87" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
@@ -8409,7 +8454,7 @@
         <v>1</v>
       </c>
       <c r="M88" s="12" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="N88" s="12">
         <v>818</v>
@@ -8419,7 +8464,7 @@
         <v>18</v>
       </c>
       <c r="P88" s="59" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="Q88" s="57">
         <f t="shared" si="10"/>
@@ -8430,7 +8475,7 @@
         <v>38</v>
       </c>
       <c r="T88" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
@@ -8463,17 +8508,17 @@
         <v>1</v>
       </c>
       <c r="M89" s="12" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="N89" s="12" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="O89" s="52" t="str">
         <f t="shared" si="12"/>
         <v>1C</v>
       </c>
       <c r="P89" s="59" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="Q89" s="57">
         <f t="shared" si="10"/>
@@ -8484,7 +8529,7 @@
         <v>39</v>
       </c>
       <c r="T89" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
@@ -8840,7 +8885,7 @@
         <v>7</v>
       </c>
       <c r="M95" s="34" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="N95" s="34">
         <v>834</v>
@@ -8903,7 +8948,7 @@
         <v>7</v>
       </c>
       <c r="M96" s="34" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="N96" s="34">
         <v>838</v>
@@ -8966,10 +9011,10 @@
         <v>7</v>
       </c>
       <c r="M97" s="34" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="N97" s="34" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="O97" s="51" t="str">
         <f t="shared" si="12"/>
@@ -9029,7 +9074,7 @@
         <v>7</v>
       </c>
       <c r="M98" s="43" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="N98" s="43">
         <v>890</v>
@@ -9051,7 +9096,7 @@
         <v>66</v>
       </c>
       <c r="T98" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="U98" s="17"/>
       <c r="V98" s="17"/>
@@ -9094,10 +9139,10 @@
         <v>7</v>
       </c>
       <c r="M99" s="43" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="N99" s="43" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="O99" s="54" t="str">
         <f t="shared" si="12"/>
@@ -9116,7 +9161,7 @@
         <v>69</v>
       </c>
       <c r="T99" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="100" spans="1:22" x14ac:dyDescent="0.25">
@@ -9157,7 +9202,7 @@
         <v>1</v>
       </c>
       <c r="M100" s="44" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="N100" s="44">
         <v>878</v>
@@ -9179,7 +9224,7 @@
         <v>60</v>
       </c>
       <c r="T100" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="101" spans="1:22" x14ac:dyDescent="0.25">
@@ -9212,10 +9257,10 @@
         <v>7</v>
       </c>
       <c r="M101" s="12" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="N101" s="12" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="O101" s="52" t="str">
         <f t="shared" si="12"/>
@@ -9233,7 +9278,7 @@
         <v>65</v>
       </c>
       <c r="T101" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="102" spans="1:22" x14ac:dyDescent="0.25">
@@ -9274,10 +9319,10 @@
         <v>7</v>
       </c>
       <c r="M102" s="83" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="N102" s="83" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="O102" s="84" t="str">
         <f t="shared" si="12"/>
@@ -9296,7 +9341,7 @@
         <v>61</v>
       </c>
       <c r="T102" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.25">
@@ -9329,7 +9374,7 @@
         <v>2</v>
       </c>
       <c r="M103" s="12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="N103" s="12">
         <v>880</v>
@@ -9339,7 +9384,7 @@
         <v>80</v>
       </c>
       <c r="P103" s="59" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="Q103" s="57">
         <f t="shared" si="10"/>
@@ -9350,7 +9395,7 @@
         <v>62</v>
       </c>
       <c r="T103" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="104" spans="1:22" x14ac:dyDescent="0.25">
@@ -9383,7 +9428,7 @@
         <v>2</v>
       </c>
       <c r="M104" s="12" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="N104" s="12">
         <v>884</v>
@@ -9393,7 +9438,7 @@
         <v>84</v>
       </c>
       <c r="P104" s="59" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="Q104" s="57">
         <f t="shared" si="10"/>
@@ -9404,7 +9449,7 @@
         <v>63</v>
       </c>
       <c r="T104" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="105" spans="1:22" x14ac:dyDescent="0.25">
@@ -9421,7 +9466,7 @@
         <v>331</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="G105" s="23" t="s">
         <v>433</v>
@@ -9442,7 +9487,7 @@
         <v>7</v>
       </c>
       <c r="M105" s="24" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="N105" s="24">
         <v>888</v>
@@ -9502,7 +9547,7 @@
         <v>7</v>
       </c>
       <c r="M106" s="43" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="N106" s="43">
         <v>894</v>
@@ -9524,7 +9569,7 @@
         <v>67</v>
       </c>
       <c r="T106" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="107" spans="1:22" x14ac:dyDescent="0.25">
@@ -9565,7 +9610,7 @@
         <v>1</v>
       </c>
       <c r="M107" s="44" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="N107" s="44">
         <v>870</v>
@@ -9587,7 +9632,7 @@
         <v>30</v>
       </c>
       <c r="T107" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="108" spans="1:22" x14ac:dyDescent="0.25">
@@ -9628,7 +9673,7 @@
         <v>7</v>
       </c>
       <c r="M108" s="43" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="N108" s="43">
         <v>898</v>
@@ -9650,7 +9695,7 @@
         <v>68</v>
       </c>
       <c r="T108" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="109" spans="1:22" x14ac:dyDescent="0.25">
@@ -9691,7 +9736,7 @@
         <v>1</v>
       </c>
       <c r="M109" s="44" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="N109" s="44">
         <v>874</v>
@@ -9713,7 +9758,7 @@
         <v>31</v>
       </c>
       <c r="T109" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="110" spans="1:22" x14ac:dyDescent="0.25">
@@ -9743,7 +9788,7 @@
         <v>0</v>
       </c>
       <c r="M110" s="12" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N110" s="12">
         <v>900</v>
@@ -9764,7 +9809,7 @@
         <v>94</v>
       </c>
       <c r="T110" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="111" spans="1:22" x14ac:dyDescent="0.25">
@@ -9794,7 +9839,7 @@
         <v>0</v>
       </c>
       <c r="M111" s="12" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="N111" s="12">
         <v>904</v>
@@ -9815,7 +9860,7 @@
         <v>95</v>
       </c>
       <c r="T111" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="112" spans="1:22" x14ac:dyDescent="0.25">
@@ -9845,10 +9890,10 @@
         <v>0</v>
       </c>
       <c r="M112" s="12" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="N112" s="12" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="O112" s="52" t="str">
         <f t="shared" si="12"/>
@@ -9866,7 +9911,7 @@
         <v>93</v>
       </c>
       <c r="T112" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
@@ -9896,10 +9941,10 @@
         <v>0</v>
       </c>
       <c r="M113" s="12" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="N113" s="12" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="O113" s="52" t="str">
         <f t="shared" si="12"/>
@@ -9917,7 +9962,7 @@
         <v>92</v>
       </c>
       <c r="T113" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
@@ -9947,10 +9992,10 @@
         <v>0</v>
       </c>
       <c r="M114" s="12" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="N114" s="12" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="O114" s="52" t="str">
         <f t="shared" si="12"/>
@@ -9968,7 +10013,7 @@
         <v>91</v>
       </c>
       <c r="T114" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="115" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9998,10 +10043,10 @@
         <v>0</v>
       </c>
       <c r="M115" s="12" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="N115" s="12" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="O115" s="55" t="str">
         <f t="shared" si="12"/>
@@ -10019,7 +10064,7 @@
         <v>90</v>
       </c>
       <c r="T115" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
   </sheetData>
@@ -10051,12 +10096,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="87" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -10069,28 +10114,28 @@
         <v>0x2F</v>
       </c>
       <c r="C3" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D3" t="str">
         <f>Sheet1!F28</f>
         <v>DOUT0</v>
       </c>
       <c r="E3" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F3" t="str">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D3),"F","G"),2,100))</f>
         <v>GPIO2_14</v>
       </c>
       <c r="G3" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H3">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D3),"F","Q"),2,100))</f>
         <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J3" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D3),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D3),"F","B"),2,100))),8)</f>
@@ -10115,28 +10160,28 @@
         <v>0x2F</v>
       </c>
       <c r="C4" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D4" t="str">
         <f>Sheet1!F29</f>
         <v>DOUT1</v>
       </c>
       <c r="E4" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4:F6" ca="1" si="2">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D4),"F","G"),2,100))</f>
         <v>GPIO2_15</v>
       </c>
       <c r="G4" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H6" ca="1" si="3">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D4),"F","Q"),2,100))</f>
         <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" ref="J4:J6" ca="1" si="4">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D4),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D4),"F","B"),2,100))),8)</f>
@@ -10161,28 +10206,28 @@
         <v>0x2F</v>
       </c>
       <c r="C5" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D5" t="str">
         <f>Sheet1!F30</f>
         <v>DOUT2</v>
       </c>
       <c r="E5" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>GPIO2_16</v>
       </c>
       <c r="G5" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="3"/>
         <v>50</v>
       </c>
       <c r="I5" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -10207,28 +10252,28 @@
         <v>0x2F</v>
       </c>
       <c r="C6" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D6" t="str">
         <f>Sheet1!F31</f>
         <v>DOUT3</v>
       </c>
       <c r="E6" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>GPIO2_17</v>
       </c>
       <c r="G6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="3"/>
         <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -10245,22 +10290,22 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="87" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -10273,28 +10318,28 @@
         <v>0x2F</v>
       </c>
       <c r="C12" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D12" t="str">
         <f>Sheet1!F20</f>
         <v>Digital Input</v>
       </c>
       <c r="E12" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ref="F12:F23" ca="1" si="7">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D12),"F","G"),2,100))</f>
         <v>GPIO2_6</v>
       </c>
       <c r="G12" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H12">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D12),"F","Q"),2,100))</f>
         <v>40</v>
       </c>
       <c r="I12" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J12" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D12),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D12),"F","B"),2,100))),8)</f>
@@ -10319,28 +10364,28 @@
         <v>0x2F</v>
       </c>
       <c r="C13" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D13" t="str">
         <f>Sheet1!F21</f>
         <v>Digital Input</v>
       </c>
       <c r="E13" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO2_7</v>
       </c>
       <c r="G13" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H13">
         <f t="shared" ref="H13:H19" ca="1" si="10">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D13),"F","Q"),2,100))</f>
         <v>41</v>
       </c>
       <c r="I13" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" ref="J13:J19" ca="1" si="11">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D13),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D13),"F","B"),2,100))),8)</f>
@@ -10365,28 +10410,28 @@
         <v>0x2F</v>
       </c>
       <c r="C14" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D14" t="str">
         <f>Sheet1!F22</f>
         <v>Digital Input</v>
       </c>
       <c r="E14" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO2_8</v>
       </c>
       <c r="G14" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
         <v>42</v>
       </c>
       <c r="I14" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -10411,28 +10456,28 @@
         <v>0x2F</v>
       </c>
       <c r="C15" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D15" t="str">
         <f>Sheet1!F23</f>
         <v>Digital Input</v>
       </c>
       <c r="E15" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO2_9</v>
       </c>
       <c r="G15" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
         <v>43</v>
       </c>
       <c r="I15" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -10457,28 +10502,28 @@
         <v>0x2F</v>
       </c>
       <c r="C16" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D16" t="str">
         <f>Sheet1!F24</f>
         <v>Digital Input</v>
       </c>
       <c r="E16" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO2_10</v>
       </c>
       <c r="G16" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
         <v>44</v>
       </c>
       <c r="I16" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -10503,28 +10548,28 @@
         <v>0x2F</v>
       </c>
       <c r="C17" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D17" t="str">
         <f>Sheet1!F25</f>
         <v>Digital Input</v>
       </c>
       <c r="E17" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO2_11</v>
       </c>
       <c r="G17" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
         <v>45</v>
       </c>
       <c r="I17" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -10549,28 +10594,28 @@
         <v>0x2F</v>
       </c>
       <c r="C18" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D18" t="str">
         <f>Sheet1!F26</f>
         <v>Digital Input</v>
       </c>
       <c r="E18" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO2_12</v>
       </c>
       <c r="G18" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
         <v>46</v>
       </c>
       <c r="I18" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -10595,28 +10640,28 @@
         <v>0x2F</v>
       </c>
       <c r="C19" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D19" t="str">
         <f>Sheet1!F27</f>
         <v>Digital Input</v>
       </c>
       <c r="E19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO2_13</v>
       </c>
       <c r="G19" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
         <v>47</v>
       </c>
       <c r="I19" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -10641,28 +10686,28 @@
         <v>0x2F</v>
       </c>
       <c r="C20" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D20" t="str">
         <f>Sheet1!F32</f>
         <v>Digital Input</v>
       </c>
       <c r="E20" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO0_8</v>
       </c>
       <c r="G20" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H20">
         <f t="shared" ref="H20" ca="1" si="16">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D20),"F","Q"),2,100))</f>
         <v>52</v>
       </c>
       <c r="I20" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" ref="J20" ca="1" si="17">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D20),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D20),"F","B"),2,100))),8)</f>
@@ -10687,28 +10732,28 @@
         <v>0x2F</v>
       </c>
       <c r="C21" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D21" t="str">
         <f>Sheet1!F33</f>
         <v>Digital Input</v>
       </c>
       <c r="E21" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO0_9</v>
       </c>
       <c r="G21" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H21">
         <f t="shared" ref="H21:H23" ca="1" si="22">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D21),"F","Q"),2,100))</f>
         <v>53</v>
       </c>
       <c r="I21" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" ref="J21:J23" ca="1" si="23">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D21),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D21),"F","B"),2,100))),8)</f>
@@ -10733,28 +10778,28 @@
         <v>0x2F</v>
       </c>
       <c r="C22" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D22" t="str">
         <f>Sheet1!F34</f>
         <v>Digital Input</v>
       </c>
       <c r="E22" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO0_10</v>
       </c>
       <c r="G22" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="22"/>
         <v>54</v>
       </c>
       <c r="I22" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" ca="1" si="23"/>
@@ -10779,28 +10824,28 @@
         <v>0x2F</v>
       </c>
       <c r="C23" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D23" t="str">
         <f>Sheet1!F35</f>
         <v>Digital Input</v>
       </c>
       <c r="E23" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>GPIO0_11</v>
       </c>
       <c r="G23" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="22"/>
         <v>55</v>
       </c>
       <c r="I23" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" ca="1" si="23"/>
@@ -10817,22 +10862,22 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="87" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -10845,28 +10890,28 @@
         <v>0x2F</v>
       </c>
       <c r="C29" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D29" t="str">
         <f>Sheet1!F36</f>
         <v>LED0</v>
       </c>
       <c r="E29" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" ref="F29:F32" ca="1" si="26">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D29),"F","G"),2,100))</f>
         <v>GPIO2_22</v>
       </c>
       <c r="G29" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H29">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D29),"F","Q"),2,100))</f>
         <v>56</v>
       </c>
       <c r="I29" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J29" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D29),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D29),"F","B"),2,100))),8)</f>
@@ -10891,28 +10936,28 @@
         <v>0x2F</v>
       </c>
       <c r="C30" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D30" t="str">
         <f>Sheet1!F37</f>
         <v>LED1</v>
       </c>
       <c r="E30" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>GPIO2_23</v>
       </c>
       <c r="G30" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H30">
         <f t="shared" ref="H30:H32" ca="1" si="29">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D30),"F","Q"),2,100))</f>
         <v>57</v>
       </c>
       <c r="I30" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" ref="J30:J32" ca="1" si="30">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D30),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D30),"F","B"),2,100))),8)</f>
@@ -10937,28 +10982,28 @@
         <v>0x2F</v>
       </c>
       <c r="C31" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D31" t="str">
         <f>Sheet1!F38</f>
         <v>LED2</v>
       </c>
       <c r="E31" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>GPIO2_24</v>
       </c>
       <c r="G31" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="29"/>
         <v>58</v>
       </c>
       <c r="I31" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" ca="1" si="30"/>
@@ -10983,28 +11028,28 @@
         <v>0x2F</v>
       </c>
       <c r="C32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D32" t="str">
         <f>Sheet1!F39</f>
         <v>LED3</v>
       </c>
       <c r="E32" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>GPIO2_25</v>
       </c>
       <c r="G32" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="29"/>
         <v>59</v>
       </c>
       <c r="I32" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" ca="1" si="30"/>
@@ -11021,22 +11066,22 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="87" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -11049,28 +11094,28 @@
         <v>0x28</v>
       </c>
       <c r="C38" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D38" t="str">
         <f>Sheet1!F62</f>
         <v>RS485</v>
       </c>
       <c r="E38" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" ref="F38:F39" ca="1" si="33">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D38),"F","G"),2,100))</f>
         <v>UART1_RXD</v>
       </c>
       <c r="G38" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H38">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D38),"F","Q"),2,100))</f>
         <v>96</v>
       </c>
       <c r="I38" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J38" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D38),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D38),"F","B"),2,100))),8)</f>
@@ -11095,28 +11140,28 @@
         <v>0x08</v>
       </c>
       <c r="C39" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D39" t="str">
         <f>Sheet1!F63</f>
         <v>RS485</v>
       </c>
       <c r="E39" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" ca="1" si="33"/>
         <v>UART1_TXD</v>
       </c>
       <c r="G39" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H39">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D39),"F","Q"),2,100))</f>
         <v>97</v>
       </c>
       <c r="I39" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J39" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D39),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D39),"F","B"),2,100))),8)</f>
@@ -11133,22 +11178,22 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="87" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -11161,28 +11206,28 @@
         <v>0x27</v>
       </c>
       <c r="C45" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D45" t="str">
         <f>Sheet1!F41</f>
         <v>DIN0</v>
       </c>
       <c r="E45" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" ref="F45:F52" ca="1" si="34">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D45),"F","G"),2,100))</f>
         <v>GPIO3_14</v>
       </c>
       <c r="G45" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H45">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D45),"F","Q"),2,100))</f>
         <v>100</v>
       </c>
       <c r="I45" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J45" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D45),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D45),"F","B"),2,100))),8)</f>
@@ -11207,28 +11252,28 @@
         <v>0x27</v>
       </c>
       <c r="C46" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D46" t="str">
         <f>Sheet1!F47</f>
         <v>DIN1</v>
       </c>
       <c r="E46" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" ca="1" si="34"/>
         <v>GPIO3_15</v>
       </c>
       <c r="G46" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H46">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D46),"F","Q"),2,100))</f>
         <v>101</v>
       </c>
       <c r="I46" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J46" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D46),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D46),"F","B"),2,100))),8)</f>
@@ -11253,28 +11298,28 @@
         <v>0x27</v>
       </c>
       <c r="C47" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D47" t="str">
         <f>Sheet1!F44</f>
         <v>DIN2</v>
       </c>
       <c r="E47" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" ca="1" si="34"/>
         <v>GPIO3_16</v>
       </c>
       <c r="G47" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H47">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D47),"F","Q"),2,100))</f>
         <v>102</v>
       </c>
       <c r="I47" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J47" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D47),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D47),"F","B"),2,100))),8)</f>
@@ -11299,28 +11344,28 @@
         <v>0x27</v>
       </c>
       <c r="C48" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D48" t="str">
         <f>Sheet1!F42</f>
         <v>DIN3</v>
       </c>
       <c r="E48" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" ca="1" si="34"/>
         <v>GPIO3_17</v>
       </c>
       <c r="G48" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H48">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D48),"F","Q"),2,100))</f>
         <v>103</v>
       </c>
       <c r="I48" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J48" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D48),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D48),"F","B"),2,100))),8)</f>
@@ -11345,28 +11390,28 @@
         <v>0x27</v>
       </c>
       <c r="C49" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D49" t="str">
         <f>Sheet1!F94</f>
         <v>DIN4</v>
       </c>
       <c r="E49" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" ca="1" si="34"/>
         <v>GPIO1_12</v>
       </c>
       <c r="G49" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H49">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D49),"F","Q"),2,100))</f>
         <v>12</v>
       </c>
       <c r="I49" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J49" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D49),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D49),"F","B"),2,100))),8)</f>
@@ -11391,28 +11436,28 @@
         <v>0x27</v>
       </c>
       <c r="C50" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D50" t="str">
         <f>Sheet1!F95</f>
         <v>DIN5</v>
       </c>
       <c r="E50" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" ca="1" si="34"/>
         <v>GPIO1_13</v>
       </c>
       <c r="G50" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H50">
         <f t="shared" ref="H50:H52" ca="1" si="39">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D50),"F","Q"),2,100))</f>
         <v>13</v>
       </c>
       <c r="I50" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" ref="J50:J52" ca="1" si="40">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D50),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D50),"F","B"),2,100))),8)</f>
@@ -11437,28 +11482,28 @@
         <v>0x27</v>
       </c>
       <c r="C51" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D51" t="str">
         <f>Sheet1!F96</f>
         <v>DIN6</v>
       </c>
       <c r="E51" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" ca="1" si="34"/>
         <v>GPIO1_14</v>
       </c>
       <c r="G51" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="39"/>
         <v>14</v>
       </c>
       <c r="I51" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" ca="1" si="40"/>
@@ -11483,28 +11528,28 @@
         <v>0x27</v>
       </c>
       <c r="C52" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D52" t="str">
         <f>Sheet1!F97</f>
         <v>DIN7</v>
       </c>
       <c r="E52" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" ca="1" si="34"/>
         <v>GPIO1_15</v>
       </c>
       <c r="G52" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="39"/>
         <v>15</v>
       </c>
       <c r="I52" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" ca="1" si="40"/>
@@ -11521,22 +11566,22 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="87" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -11549,28 +11594,28 @@
         <v>0x0F</v>
       </c>
       <c r="C57" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D57" t="str">
         <f>Sheet1!F98</f>
         <v>Relay0</v>
       </c>
       <c r="E57" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" ref="F57:F60" ca="1" si="43">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D57),"F","G"),2,100))</f>
         <v>GPIO2_2</v>
       </c>
       <c r="G57" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H57">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D57),"F","Q"),2,100))</f>
         <v>36</v>
       </c>
       <c r="I57" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J57" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D57),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D57),"F","B"),2,100))),8)</f>
@@ -11595,28 +11640,28 @@
         <v>0x0F</v>
       </c>
       <c r="C58" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D58" t="str">
         <f>Sheet1!F106</f>
         <v>Relay1</v>
       </c>
       <c r="E58" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" ca="1" si="43"/>
         <v>GPIO2_3</v>
       </c>
       <c r="G58" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H58">
         <f t="shared" ref="H58:H60" ca="1" si="46">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D58),"F","Q"),2,100))</f>
         <v>37</v>
       </c>
       <c r="I58" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" ref="J58:J60" ca="1" si="47">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D58),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D58),"F","B"),2,100))),8)</f>
@@ -11641,28 +11686,28 @@
         <v>0x0F</v>
       </c>
       <c r="C59" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D59" t="str">
         <f>Sheet1!F108</f>
         <v>Relay2</v>
       </c>
       <c r="E59" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" ca="1" si="43"/>
         <v>GPIO2_4</v>
       </c>
       <c r="G59" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="46"/>
         <v>38</v>
       </c>
       <c r="I59" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -11687,28 +11732,28 @@
         <v>0x0F</v>
       </c>
       <c r="C60" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D60" t="str">
         <f>Sheet1!F99</f>
         <v>Relay3</v>
       </c>
       <c r="E60" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" ca="1" si="43"/>
         <v>GPIO2_5</v>
       </c>
       <c r="G60" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="46"/>
         <v>39</v>
       </c>
       <c r="I60" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -11725,22 +11770,22 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="87" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -11753,28 +11798,28 @@
         <v>0x34</v>
       </c>
       <c r="C66" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D66" t="str">
         <f>Sheet1!F46</f>
         <v>JTAG_EMU2</v>
       </c>
       <c r="E66" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F66" t="str">
         <f t="shared" ref="F66" ca="1" si="52">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D66),"F","G"),2,100))</f>
         <v>EMU2</v>
       </c>
       <c r="G66" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H66">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D66),"F","Q"),2,100))</f>
         <v>105</v>
       </c>
       <c r="I66" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J66" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D66),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D66),"F","B"),2,100))),8)</f>
@@ -11791,22 +11836,22 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="87" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -11819,28 +11864,28 @@
         <v>0x27</v>
       </c>
       <c r="C72" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D72" t="str">
         <f>Sheet1!F68</f>
         <v>RTC_INT</v>
       </c>
       <c r="E72" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" ref="F72" ca="1" si="55">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D72),"F","G"),2,100))</f>
         <v>GPIO0_19</v>
       </c>
       <c r="G72" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H72">
         <f t="shared" ref="H72" ca="1" si="56">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D72),"F","Q"),2,100))</f>
         <v>108</v>
       </c>
       <c r="I72" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J72" t="str">
         <f t="shared" ref="J72" ca="1" si="57">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D72),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D72),"F","B"),2,100))),8)</f>
@@ -11857,22 +11902,22 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="87" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -11885,28 +11930,28 @@
         <v>0x0F</v>
       </c>
       <c r="C78" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D78" t="str">
         <f>Sheet1!F102</f>
         <v>EMMC_RST_INT</v>
       </c>
       <c r="E78" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" ref="F78" ca="1" si="62">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D78),"F","G"),2,100))</f>
         <v>GPIO1_29</v>
       </c>
       <c r="G78" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H78">
         <f t="shared" ref="H78" ca="1" si="63">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D78),"F","Q"),2,100))</f>
         <v>31</v>
       </c>
       <c r="I78" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J78" t="str">
         <f t="shared" ref="J78" ca="1" si="64">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D78),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D78),"F","B"),2,100))),8)</f>
@@ -11923,22 +11968,22 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="87" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -11951,28 +11996,28 @@
         <v>0x01</v>
       </c>
       <c r="C84" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D84" t="str">
         <f>Sheet1!F70</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E84" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" ref="F84:F98" ca="1" si="69">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D84),"F","G"),2,100))</f>
         <v>GMII2_TXEN</v>
       </c>
       <c r="G84" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H84">
         <f t="shared" ref="H84" ca="1" si="70">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D84),"F","Q"),2,100))</f>
         <v>16</v>
       </c>
       <c r="I84" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J84" t="str">
         <f t="shared" ref="J84" ca="1" si="71">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D84),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D84),"F","B"),2,100))),8)</f>
@@ -11997,28 +12042,28 @@
         <v>0x21</v>
       </c>
       <c r="C85" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D85" t="str">
         <f>Sheet1!F71</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E85" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_RXDV</v>
       </c>
       <c r="G85" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H85">
         <f t="shared" ref="H85:H104" ca="1" si="76">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D85),"F","Q"),2,100))</f>
         <v>17</v>
       </c>
       <c r="I85" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J85" t="str">
         <f t="shared" ref="J85:J104" ca="1" si="77">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D85),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D85),"F","B"),2,100))),8)</f>
@@ -12043,28 +12088,28 @@
         <v>0x01</v>
       </c>
       <c r="C86" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D86" t="str">
         <f>Sheet1!F72</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E86" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_TXD3</v>
       </c>
       <c r="G86" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="76"/>
         <v>18</v>
       </c>
       <c r="I86" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J86" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12089,28 +12134,28 @@
         <v>0x01</v>
       </c>
       <c r="C87" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D87" t="str">
         <f>Sheet1!F73</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E87" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_TXD2</v>
       </c>
       <c r="G87" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="76"/>
         <v>19</v>
       </c>
       <c r="I87" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J87" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12135,28 +12180,28 @@
         <v>0x01</v>
       </c>
       <c r="C88" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D88" t="str">
         <f>Sheet1!F74</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E88" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_TXD1</v>
       </c>
       <c r="G88" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="76"/>
         <v>20</v>
       </c>
       <c r="I88" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J88" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12181,28 +12226,28 @@
         <v>0x01</v>
       </c>
       <c r="C89" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D89" t="str">
         <f>Sheet1!F75</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E89" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_TXD0</v>
       </c>
       <c r="G89" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="76"/>
         <v>21</v>
       </c>
       <c r="I89" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J89" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12227,28 +12272,28 @@
         <v>0x21</v>
       </c>
       <c r="C90" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D90" t="str">
         <f>Sheet1!F76</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E90" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_TXCLK</v>
       </c>
       <c r="G90" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H90">
         <f t="shared" ca="1" si="76"/>
         <v>22</v>
       </c>
       <c r="I90" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J90" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12273,28 +12318,28 @@
         <v>0x21</v>
       </c>
       <c r="C91" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D91" t="str">
         <f>Sheet1!F77</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E91" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_RXCLK</v>
       </c>
       <c r="G91" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H91">
         <f t="shared" ca="1" si="76"/>
         <v>23</v>
       </c>
       <c r="I91" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J91" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12319,28 +12364,28 @@
         <v>0x21</v>
       </c>
       <c r="C92" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D92" t="str">
         <f>Sheet1!F78</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E92" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_RXD3</v>
       </c>
       <c r="G92" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="76"/>
         <v>24</v>
       </c>
       <c r="I92" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J92" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12365,28 +12410,28 @@
         <v>0x21</v>
       </c>
       <c r="C93" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D93" t="str">
         <f>Sheet1!F79</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E93" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_RXD2</v>
       </c>
       <c r="G93" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H93">
         <f t="shared" ca="1" si="76"/>
         <v>25</v>
       </c>
       <c r="I93" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J93" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12411,28 +12456,28 @@
         <v>0x21</v>
       </c>
       <c r="C94" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D94" t="str">
         <f>Sheet1!F80</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E94" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_RXD1</v>
       </c>
       <c r="G94" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="76"/>
         <v>26</v>
       </c>
       <c r="I94" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J94" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12457,28 +12502,28 @@
         <v>0x21</v>
       </c>
       <c r="C95" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D95" t="str">
         <f>Sheet1!F81</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E95" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_RXD0</v>
       </c>
       <c r="G95" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="76"/>
         <v>27</v>
       </c>
       <c r="I95" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J95" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12503,28 +12548,28 @@
         <v>0x29</v>
       </c>
       <c r="C96" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D96" t="str">
         <f>Sheet1!F100</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E96" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_COL</v>
       </c>
       <c r="G96" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H96">
         <f t="shared" ca="1" si="76"/>
         <v>30</v>
       </c>
       <c r="I96" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J96" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12549,28 +12594,28 @@
         <v>0x29</v>
       </c>
       <c r="C97" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D97" t="str">
         <f>Sheet1!F107</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E97" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_CRS</v>
       </c>
       <c r="G97" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="76"/>
         <v>28</v>
       </c>
       <c r="I97" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J97" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12595,28 +12640,28 @@
         <v>0x21</v>
       </c>
       <c r="C98" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D98" t="str">
         <f>Sheet1!F109</f>
         <v>Ethernet 2nd module</v>
       </c>
       <c r="E98" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" ca="1" si="69"/>
         <v>GMII2_RXERR</v>
       </c>
       <c r="G98" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="76"/>
         <v>29</v>
       </c>
       <c r="I98" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J98" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12633,22 +12678,22 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="87" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="87" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
@@ -12661,28 +12706,28 @@
         <v>0x27</v>
       </c>
       <c r="C104" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D104" t="str">
         <f>Sheet1!F40</f>
         <v>TP41</v>
       </c>
       <c r="E104" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" ref="F104:F115" ca="1" si="80">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D104),"F","G"),2,100))</f>
         <v>GPIO3_18</v>
       </c>
       <c r="G104" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H104">
         <f t="shared" ca="1" si="76"/>
         <v>104</v>
       </c>
       <c r="I104" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J104" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -12707,28 +12752,28 @@
         <v>0x27</v>
       </c>
       <c r="C105" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D105" t="str">
         <f>Sheet1!F43</f>
         <v>TP36</v>
       </c>
       <c r="E105" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO3_21</v>
       </c>
       <c r="G105" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H105">
         <f t="shared" ref="H105:H111" ca="1" si="83">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D105),"F","Q"),2,100))</f>
         <v>107</v>
       </c>
       <c r="I105" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J105" t="str">
         <f t="shared" ref="J105:J111" ca="1" si="84">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D105),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D105),"F","B"),2,100))),8)</f>
@@ -12753,28 +12798,28 @@
         <v>0x27</v>
       </c>
       <c r="C106" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D106" t="str">
         <f>Sheet1!F53</f>
         <v>TP32</v>
       </c>
       <c r="E106" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO0_3</v>
       </c>
       <c r="G106" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H106">
         <f t="shared" ca="1" si="83"/>
         <v>85</v>
       </c>
       <c r="I106" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J106" t="str">
         <f t="shared" ca="1" si="84"/>
@@ -12786,7 +12831,7 @@
       </c>
       <c r="L106" t="str">
         <f t="shared" ca="1" si="86"/>
-        <v>slew=fast,I/O,pulldown,mode=7</v>
+        <v>slew=fast,I/O,pull disabled,mode=7</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -12799,28 +12844,28 @@
         <v>0x27</v>
       </c>
       <c r="C107" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D107" t="str">
         <f>Sheet1!F55</f>
         <v>TP31</v>
       </c>
       <c r="E107" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO0_2</v>
       </c>
       <c r="G107" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H107">
         <f t="shared" ca="1" si="83"/>
         <v>84</v>
       </c>
       <c r="I107" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J107" t="str">
         <f t="shared" ca="1" si="84"/>
@@ -12845,28 +12890,28 @@
         <v>0x27</v>
       </c>
       <c r="C108" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D108" t="str">
         <f>Sheet1!F57</f>
         <v>TP33</v>
       </c>
       <c r="E108" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO1_9</v>
       </c>
       <c r="G108" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H108">
         <f t="shared" ca="1" si="83"/>
         <v>91</v>
       </c>
       <c r="I108" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J108" t="str">
         <f t="shared" ca="1" si="84"/>
@@ -12891,28 +12936,28 @@
         <v>0x73</v>
       </c>
       <c r="C109" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D109" t="str">
         <f>Sheet1!F60</f>
         <v>TP34</v>
       </c>
       <c r="E109" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO0_12</v>
       </c>
       <c r="G109" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H109">
         <f t="shared" ca="1" si="83"/>
         <v>94</v>
       </c>
       <c r="I109" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J109" t="str">
         <f t="shared" ca="1" si="84"/>
@@ -12937,28 +12982,28 @@
         <v>0x73</v>
       </c>
       <c r="C110" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D110" t="str">
         <f>Sheet1!F61</f>
         <v>TP35</v>
       </c>
       <c r="E110" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO0_13</v>
       </c>
       <c r="G110" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H110">
         <f t="shared" ca="1" si="83"/>
         <v>95</v>
       </c>
       <c r="I110" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J110" t="str">
         <f t="shared" ca="1" si="84"/>
@@ -12983,28 +13028,28 @@
         <v>0x27</v>
       </c>
       <c r="C111" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D111" t="str">
         <f>Sheet1!F90</f>
         <v>TP23</v>
       </c>
       <c r="E111" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO0_22</v>
       </c>
       <c r="G111" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H111">
         <f t="shared" ca="1" si="83"/>
         <v>8</v>
       </c>
       <c r="I111" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J111" t="str">
         <f t="shared" ca="1" si="84"/>
@@ -13029,28 +13074,28 @@
         <v>0x27</v>
       </c>
       <c r="C112" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D112" t="str">
         <f>Sheet1!F91</f>
         <v>TP24</v>
       </c>
       <c r="E112" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO0_23</v>
       </c>
       <c r="G112" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H112">
         <f t="shared" ref="H112:H114" ca="1" si="89">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D112),"F","Q"),2,100))</f>
         <v>9</v>
       </c>
       <c r="I112" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J112" t="str">
         <f t="shared" ref="J112:J114" ca="1" si="90">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D112),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D112),"F","B"),2,100))),8)</f>
@@ -13075,28 +13120,28 @@
         <v>0x27</v>
       </c>
       <c r="C113" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D113" t="str">
         <f>Sheet1!F92</f>
         <v>TP25</v>
       </c>
       <c r="E113" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F113" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO0_26</v>
       </c>
       <c r="G113" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H113">
         <f t="shared" ca="1" si="89"/>
         <v>10</v>
       </c>
       <c r="I113" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J113" t="str">
         <f t="shared" ca="1" si="90"/>
@@ -13121,28 +13166,28 @@
         <v>0x27</v>
       </c>
       <c r="C114" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D114" t="str">
         <f>Sheet1!F93</f>
         <v>TP26</v>
       </c>
       <c r="E114" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F114" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO0_27</v>
       </c>
       <c r="G114" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H114">
         <f t="shared" ca="1" si="89"/>
         <v>11</v>
       </c>
       <c r="I114" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J114" t="str">
         <f t="shared" ca="1" si="90"/>
@@ -13167,28 +13212,28 @@
         <v>0x27</v>
       </c>
       <c r="C115" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D115" t="str">
         <f>Sheet1!F105</f>
         <v>TP29</v>
       </c>
       <c r="E115" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F115" t="str">
         <f t="shared" ca="1" si="80"/>
         <v>GPIO2_0</v>
       </c>
       <c r="G115" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H115">
         <f ca="1">INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D115),"F","Q"),2,100))</f>
         <v>34</v>
       </c>
       <c r="I115" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J115" t="str">
         <f ca="1">MID( INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D115),"F","B"),2,100)),FIND("GPIO", INDIRECT(MID(SUBSTITUTE(_xlfn.FORMULATEXT(D115),"F","B"),2,100))),8)</f>
@@ -13205,12 +13250,12 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>